<commit_message>
Check for changes in the LocationAPI database
</commit_message>
<xml_diff>
--- a/data/data_comparison.xlsx
+++ b/data/data_comparison.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\PycharmProjects\Localization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\PycharmProjects\Localization\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8508"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8508" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Mean + median errors" sheetId="1" r:id="rId1"/>
     <sheet name="Chance of match" sheetId="2" r:id="rId2"/>
+    <sheet name="LocationAPI - with(out) RSSI" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Location</t>
   </si>
@@ -59,17 +60,39 @@
   <si>
     <t>Mean3</t>
   </si>
+  <si>
+    <t>LocationAPI with RSSI mean error (km)</t>
+  </si>
+  <si>
+    <t>LocationAPI without RSSI mean error (km)</t>
+  </si>
+  <si>
+    <t>LocationAPI with RSSI median error (km)</t>
+  </si>
+  <si>
+    <t>LocationAPI without RSSI median error (km)</t>
+  </si>
+  <si>
+    <t>Extreme value</t>
+  </si>
+  <si>
+    <t>Different value</t>
+  </si>
+  <si>
+    <t>Best value</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="&quot;BAP &quot;\ 0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,8 +136,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,8 +181,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -221,13 +268,100 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -257,13 +391,564 @@
     <xf numFmtId="166" fontId="2" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="4" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="4"/>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="7" fillId="7" borderId="7" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="7" fillId="7" borderId="10" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="7" fillId="7" borderId="9" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="7" fillId="7" borderId="13" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="7" fillId="7" borderId="3" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="60% - Accent6" xfId="2" builtinId="52"/>
     <cellStyle name="Goed" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutraal" xfId="4" builtinId="28"/>
+    <cellStyle name="Ongeldig" xfId="3" builtinId="27"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="46">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0000"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0000"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="0.0000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color theme="0"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="0.0000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color theme="0"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="0.0000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color theme="0"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="0.0000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="&quot;BAP &quot;\ 0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="&quot;BAP &quot;\ 0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -624,106 +1309,6 @@
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -6027,35 +6612,49 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel2" displayName="Tabel2" ref="A1:E38" totalsRowCount="1" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel2" displayName="Tabel2" ref="A1:E38" totalsRowCount="1" tableBorderDxfId="45" totalsRowBorderDxfId="44">
   <autoFilter ref="A1:E37"/>
   <sortState ref="A2:E37">
     <sortCondition ref="A1:A37"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="Location" totalsRowLabel="Mean" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="2" name="WiGLE mean error (km)" totalsRowFunction="average" dataDxfId="13" totalsRowDxfId="12" totalsRowCellStyle="Goed"/>
-    <tableColumn id="3" name="LocationAPI mean error (km)" totalsRowFunction="average" totalsRowDxfId="11" dataCellStyle="Goed" totalsRowCellStyle="Standaard"/>
-    <tableColumn id="4" name="WiGLE median error (km)" totalsRowFunction="average" dataDxfId="10" totalsRowDxfId="9"/>
-    <tableColumn id="5" name="LocationAPI median error (km)" totalsRowFunction="average" totalsRowDxfId="8" totalsRowCellStyle="Goed"/>
+    <tableColumn id="1" name="Location" totalsRowLabel="Mean" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="2" name="WiGLE mean error (km)" totalsRowFunction="average" dataDxfId="41" totalsRowDxfId="40" totalsRowCellStyle="Goed"/>
+    <tableColumn id="3" name="LocationAPI mean error (km)" totalsRowFunction="average" totalsRowDxfId="39" dataCellStyle="Goed" totalsRowCellStyle="Standaard"/>
+    <tableColumn id="4" name="WiGLE median error (km)" totalsRowFunction="average" dataDxfId="38" totalsRowDxfId="37"/>
+    <tableColumn id="5" name="LocationAPI median error (km)" totalsRowFunction="average" totalsRowDxfId="36" totalsRowCellStyle="Goed"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:G38" totalsRowShown="0" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:G38" totalsRowShown="0" dataDxfId="35">
   <autoFilter ref="A1:G38"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Location" dataDxfId="6"/>
-    <tableColumn id="2" name="WiGLE chance of BSSID match (%)" dataDxfId="5"/>
-    <tableColumn id="5" name="Mean" dataDxfId="4"/>
-    <tableColumn id="3" name="WiGLE 2 BSSIDs not found (%)" dataDxfId="3"/>
-    <tableColumn id="6" name="Mean2" dataDxfId="2" dataCellStyle="60% - Accent6"/>
-    <tableColumn id="4" name="LocationAPI 2 BSSIDs not found (%)" dataDxfId="1"/>
-    <tableColumn id="7" name="Mean3" dataDxfId="0"/>
+    <tableColumn id="1" name="Location" dataDxfId="34"/>
+    <tableColumn id="2" name="WiGLE chance of BSSID match (%)" dataDxfId="33"/>
+    <tableColumn id="5" name="Mean" dataDxfId="32"/>
+    <tableColumn id="3" name="WiGLE 2 BSSIDs not found (%)" dataDxfId="31"/>
+    <tableColumn id="6" name="Mean2" dataDxfId="30" dataCellStyle="60% - Accent6"/>
+    <tableColumn id="4" name="LocationAPI 2 BSSIDs not found (%)" dataDxfId="29"/>
+    <tableColumn id="7" name="Mean3" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel3" displayName="Tabel3" ref="A1:E38" totalsRowCount="1" headerRowDxfId="13" dataDxfId="12" headerRowBorderDxfId="11">
+  <autoFilter ref="A1:E37"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Location" totalsRowLabel="Mean" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="2" name="LocationAPI with RSSI mean error (km)" totalsRowFunction="average" dataDxfId="8" totalsRowDxfId="3" totalsRowCellStyle="Neutraal"/>
+    <tableColumn id="3" name="LocationAPI without RSSI mean error (km)" totalsRowFunction="average" dataDxfId="4" totalsRowDxfId="2" totalsRowCellStyle="Neutraal"/>
+    <tableColumn id="4" name="LocationAPI with RSSI median error (km)" totalsRowFunction="average" dataDxfId="6" totalsRowDxfId="1" totalsRowCellStyle="Neutraal"/>
+    <tableColumn id="5" name="LocationAPI without RSSI median error (km)" totalsRowFunction="average" dataDxfId="5" totalsRowDxfId="0" totalsRowCellStyle="Neutraal"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -6356,10 +6955,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6373,9 +6972,10 @@
     <col min="7" max="7" width="17.21875" customWidth="1"/>
     <col min="8" max="8" width="15.77734375" customWidth="1"/>
     <col min="9" max="9" width="15.5546875" customWidth="1"/>
+    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -6392,7 +6992,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -6408,8 +7008,11 @@
       <c r="E2" s="6">
         <v>2.2963518229667992E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="P2" s="37" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -6425,8 +7028,11 @@
       <c r="E3" s="6">
         <v>5.8544262287531769E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="P3" s="36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -6443,7 +7049,7 @@
         <v>0.30805396715219591</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -6460,7 +7066,7 @@
         <v>6.4528522437704669E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -6477,7 +7083,7 @@
         <v>2.73776840170065E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -6494,7 +7100,7 @@
         <v>1.3113749685182309E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -6511,7 +7117,7 @@
         <v>2.270711644424948E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -6528,7 +7134,7 @@
         <v>3.710694621264924E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -6545,7 +7151,7 @@
         <v>0.17294743318736339</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -6562,7 +7168,7 @@
         <v>3.5847624697633446E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -6579,7 +7185,7 @@
         <v>6.2981399718856759E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -6596,7 +7202,7 @@
         <v>4.4597081552155853E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -6613,7 +7219,7 @@
         <v>5.5727207882154878E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -6630,7 +7236,7 @@
         <v>2.0758705629549509E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -7089,8 +7695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7983,4 +8589,707 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.44140625" customWidth="1"/>
+    <col min="2" max="2" width="35.44140625" customWidth="1"/>
+    <col min="3" max="4" width="38.33203125" customWidth="1"/>
+    <col min="5" max="5" width="41" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="27">
+        <v>546.38786479147541</v>
+      </c>
+      <c r="C2" s="30">
+        <v>546.38786479147495</v>
+      </c>
+      <c r="D2" s="30">
+        <v>2.2963518229667992E-2</v>
+      </c>
+      <c r="E2" s="30">
+        <v>2.2963518229667992E-2</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="28">
+        <v>6.6589453826347497E-2</v>
+      </c>
+      <c r="C3" s="31">
+        <v>6.7508700279675579E-2</v>
+      </c>
+      <c r="D3" s="30">
+        <v>5.8544262287531769E-2</v>
+      </c>
+      <c r="E3" s="30">
+        <v>5.8544262287531769E-2</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="27">
+        <v>0.31081984144760638</v>
+      </c>
+      <c r="C4" s="30">
+        <v>0.31081984144760638</v>
+      </c>
+      <c r="D4" s="30">
+        <v>0.30805396715219591</v>
+      </c>
+      <c r="E4" s="30">
+        <v>0.30805396715219591</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="28">
+        <v>6.75349237985714E-2</v>
+      </c>
+      <c r="C5" s="31">
+        <v>6.7684447273782491E-2</v>
+      </c>
+      <c r="D5" s="31">
+        <v>6.4528522437704669E-2</v>
+      </c>
+      <c r="E5" s="31">
+        <v>6.4929687360808092E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="27">
+        <v>2.2467670715647552</v>
+      </c>
+      <c r="C6" s="30">
+        <v>2.2467670715647552</v>
+      </c>
+      <c r="D6" s="30">
+        <v>2.73776840170065E-2</v>
+      </c>
+      <c r="E6" s="30">
+        <v>2.73776840170065E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="28">
+        <v>1.7181463681379079E-2</v>
+      </c>
+      <c r="C7" s="31">
+        <v>1.5458090292626001E-2</v>
+      </c>
+      <c r="D7" s="31">
+        <v>1.3113749685182309E-2</v>
+      </c>
+      <c r="E7" s="31">
+        <v>1.5691085358153091E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="28">
+        <v>2.523377474158545E-2</v>
+      </c>
+      <c r="C8" s="31">
+        <v>2.579172889491679E-2</v>
+      </c>
+      <c r="D8" s="30">
+        <v>2.270711644424948E-2</v>
+      </c>
+      <c r="E8" s="30">
+        <v>2.270711644424948E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="27">
+        <v>4.2604164317743352E-2</v>
+      </c>
+      <c r="C9" s="30">
+        <v>4.2604164317743352E-2</v>
+      </c>
+      <c r="D9" s="30">
+        <v>3.710694621264924E-2</v>
+      </c>
+      <c r="E9" s="30">
+        <v>3.710694621264924E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="28">
+        <v>0.16779120910126999</v>
+      </c>
+      <c r="C10" s="31">
+        <v>0.1630582383899318</v>
+      </c>
+      <c r="D10" s="31">
+        <v>0.17294743318736339</v>
+      </c>
+      <c r="E10" s="31">
+        <v>0.16233527625047309</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="28">
+        <v>4.0055828890416499E-2</v>
+      </c>
+      <c r="C11" s="31">
+        <v>3.6925145765380543E-2</v>
+      </c>
+      <c r="D11" s="31">
+        <v>3.5847624697633446E-2</v>
+      </c>
+      <c r="E11" s="31">
+        <v>3.2558574752882707E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="28">
+        <v>7.7630827700998273E-2</v>
+      </c>
+      <c r="C12" s="31">
+        <v>6.4277820153357132E-2</v>
+      </c>
+      <c r="D12" s="31">
+        <v>6.2981399718856759E-2</v>
+      </c>
+      <c r="E12" s="31">
+        <v>6.1840837056184733E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="28">
+        <v>4.4704625976817368E-2</v>
+      </c>
+      <c r="C13" s="31">
+        <v>4.5296107161432078E-2</v>
+      </c>
+      <c r="D13" s="31">
+        <v>4.4597081552155853E-2</v>
+      </c>
+      <c r="E13" s="31">
+        <v>3.6608694278261328E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="27">
+        <v>1.9077187438057179</v>
+      </c>
+      <c r="C14" s="30">
+        <v>1.9077187438057179</v>
+      </c>
+      <c r="D14" s="30">
+        <v>5.5727207882154878E-2</v>
+      </c>
+      <c r="E14" s="30">
+        <v>5.5727207882154878E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="27">
+        <v>2.3659057236574479E-2</v>
+      </c>
+      <c r="C15" s="30">
+        <v>2.3659057236574479E-2</v>
+      </c>
+      <c r="D15" s="30">
+        <v>2.0758705629549509E-2</v>
+      </c>
+      <c r="E15" s="30">
+        <v>2.0758705629549509E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="28">
+        <v>5.0776323191418303E-2</v>
+      </c>
+      <c r="C16" s="31">
+        <v>3.893424249758428E-2</v>
+      </c>
+      <c r="D16" s="31">
+        <v>4.8382735876750647E-2</v>
+      </c>
+      <c r="E16" s="31">
+        <v>3.6557797618095036E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="27">
+        <v>4.8740845352458151E-2</v>
+      </c>
+      <c r="C17" s="30">
+        <v>4.8740845352458151E-2</v>
+      </c>
+      <c r="D17" s="30">
+        <v>3.883072403776161E-2</v>
+      </c>
+      <c r="E17" s="30">
+        <v>3.883072403776161E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="28">
+        <v>0.21899005151813941</v>
+      </c>
+      <c r="C18" s="31">
+        <v>4.8933393131479527E-2</v>
+      </c>
+      <c r="D18" s="31">
+        <v>4.358991946510065E-2</v>
+      </c>
+      <c r="E18" s="31">
+        <v>4.4653914860836197E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="27">
+        <v>6.1523920674473327E-2</v>
+      </c>
+      <c r="C19" s="30">
+        <v>6.1523920674473327E-2</v>
+      </c>
+      <c r="D19" s="30">
+        <v>5.0269067311446723E-2</v>
+      </c>
+      <c r="E19" s="30">
+        <v>5.0269067311446723E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="28">
+        <v>4.3399808422187283E-2</v>
+      </c>
+      <c r="C20" s="31">
+        <v>4.3257634327963798E-2</v>
+      </c>
+      <c r="D20" s="30">
+        <v>4.4336515176840202E-2</v>
+      </c>
+      <c r="E20" s="30">
+        <v>4.4336515176840202E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="28">
+        <v>3.8577956147864592E-2</v>
+      </c>
+      <c r="C21" s="31">
+        <v>3.7930646256254898E-2</v>
+      </c>
+      <c r="D21" s="30">
+        <v>2.8742163613464201E-2</v>
+      </c>
+      <c r="E21" s="30">
+        <v>2.8742163613464201E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="28">
+        <v>3.9541356031615189E-2</v>
+      </c>
+      <c r="C22" s="31">
+        <v>3.8610859221155432E-2</v>
+      </c>
+      <c r="D22" s="31">
+        <v>3.5628454750964662E-2</v>
+      </c>
+      <c r="E22" s="31">
+        <v>3.3334472749350988E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="28">
+        <v>4.1108137227847541</v>
+      </c>
+      <c r="C23" s="31">
+        <v>1.4510001727621571</v>
+      </c>
+      <c r="D23" s="31">
+        <v>4.3063385848842825E-2</v>
+      </c>
+      <c r="E23" s="31">
+        <v>3.6947996248945639E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="27">
+        <v>8.6846575250509331E-2</v>
+      </c>
+      <c r="C24" s="30">
+        <v>8.6846575250509331E-2</v>
+      </c>
+      <c r="D24" s="30">
+        <v>8.1037218864693797E-2</v>
+      </c>
+      <c r="E24" s="30">
+        <v>8.1037218864693797E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="27">
+        <v>10.2055248780983</v>
+      </c>
+      <c r="C25" s="30">
+        <v>10.2055248780983</v>
+      </c>
+      <c r="D25" s="30">
+        <v>8.7838087348634006E-2</v>
+      </c>
+      <c r="E25" s="30">
+        <v>8.7838087348634006E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="27">
+        <v>1.965581555301946E-2</v>
+      </c>
+      <c r="C26" s="30">
+        <v>1.965581555301946E-2</v>
+      </c>
+      <c r="D26" s="30">
+        <v>1.7671811392270621E-2</v>
+      </c>
+      <c r="E26" s="30">
+        <v>1.7671811392270621E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="27">
+        <v>4.7616282868674489E-2</v>
+      </c>
+      <c r="C27" s="30">
+        <v>4.7616282868674489E-2</v>
+      </c>
+      <c r="D27" s="30">
+        <v>4.3173697986620796E-2</v>
+      </c>
+      <c r="E27" s="30">
+        <v>4.3173697986620796E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="28">
+        <v>4.6439693993404037E-2</v>
+      </c>
+      <c r="C28" s="31">
+        <v>4.8338039186879282E-2</v>
+      </c>
+      <c r="D28" s="31">
+        <v>3.9782807177896902E-2</v>
+      </c>
+      <c r="E28" s="31">
+        <v>4.2009666844848061E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="28">
+        <v>5.3188907899153801E-2</v>
+      </c>
+      <c r="C29" s="31">
+        <v>5.1441372574987668E-2</v>
+      </c>
+      <c r="D29" s="31">
+        <v>4.9081688292464259E-2</v>
+      </c>
+      <c r="E29" s="31">
+        <v>4.840450380244337E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="28">
+        <v>0.2722447537588471</v>
+      </c>
+      <c r="C30" s="31">
+        <v>0.27196085285516208</v>
+      </c>
+      <c r="D30" s="31">
+        <v>4.3665588408730027E-2</v>
+      </c>
+      <c r="E30" s="31">
+        <v>4.4409305118097139E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="28">
+        <v>2.50015373576042E-2</v>
+      </c>
+      <c r="C31" s="31">
+        <v>2.540145694882423E-2</v>
+      </c>
+      <c r="D31" s="31">
+        <v>2.2248419911489559E-2</v>
+      </c>
+      <c r="E31" s="31">
+        <v>2.2945301714554809E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="28">
+        <v>6.5363042605087864</v>
+      </c>
+      <c r="C32" s="31">
+        <v>6.5338109722380606</v>
+      </c>
+      <c r="D32" s="31">
+        <v>3.7989621013067493E-2</v>
+      </c>
+      <c r="E32" s="31">
+        <v>3.6810921495245744E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="28">
+        <v>0.1199194010314637</v>
+      </c>
+      <c r="C33" s="31">
+        <v>0.12089671764559989</v>
+      </c>
+      <c r="D33" s="31">
+        <v>0.1044433098927853</v>
+      </c>
+      <c r="E33" s="31">
+        <v>0.1054239517201123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="27">
+        <v>4.4541066152575998E-2</v>
+      </c>
+      <c r="C34" s="30">
+        <v>4.4541066152575998E-2</v>
+      </c>
+      <c r="D34" s="30">
+        <v>3.796387400858528E-2</v>
+      </c>
+      <c r="E34" s="30">
+        <v>3.796387400858528E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="27">
+        <v>2.5581608712796501E-2</v>
+      </c>
+      <c r="C35" s="30">
+        <v>2.5581608712796501E-2</v>
+      </c>
+      <c r="D35" s="30">
+        <v>2.1730259127721412E-2</v>
+      </c>
+      <c r="E35" s="30">
+        <v>2.1730259127721412E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="28">
+        <v>1.3142008187728709E-2</v>
+      </c>
+      <c r="C36" s="31">
+        <v>1.539060874652811E-2</v>
+      </c>
+      <c r="D36" s="31">
+        <v>1.563338138862146E-2</v>
+      </c>
+      <c r="E36" s="31">
+        <v>1.6589648080492361E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>36</v>
+      </c>
+      <c r="B37" s="33">
+        <v>0.14525513124737119</v>
+      </c>
+      <c r="C37" s="34">
+        <v>2.1920824388186742E-2</v>
+      </c>
+      <c r="D37" s="34">
+        <v>9.9956408058352684E-3</v>
+      </c>
+      <c r="E37" s="34">
+        <v>1.1002763469003101E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="35">
+        <f>SUBTOTAL(101,Tabel3[LocationAPI with RSSI mean error (km)])</f>
+        <v>15.935549491175237</v>
+      </c>
+      <c r="C38" s="35">
+        <f>SUBTOTAL(101,Tabel3[LocationAPI without RSSI mean error (km)])</f>
+        <v>15.852591464819502</v>
+      </c>
+      <c r="D38" s="35">
+        <f>SUBTOTAL(101,Tabel3[LocationAPI with RSSI median error (km)])</f>
+        <v>5.2565377523180253E-2</v>
+      </c>
+      <c r="E38" s="35">
+        <f>SUBTOTAL(101,Tabel3[LocationAPI without RSSI median error (km)])</f>
+        <v>5.1607978486161984E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D2:D37">
+    <cfRule type="cellIs" dxfId="17" priority="5" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C37">
+    <cfRule type="cellIs" dxfId="16" priority="7" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B37 B4:C37">
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E37">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Calculate error of 2 BSSIDs with highest RSSI values (LocationAPI without RSSI in request)
</commit_message>
<xml_diff>
--- a/data/data_comparison.xlsx
+++ b/data/data_comparison.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
   <si>
     <t>Location</t>
   </si>
@@ -5134,20 +5134,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.109375" style="53" customWidth="1"/>
     <col min="2" max="2" width="42.5546875" style="53" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.88671875" style="53" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.5546875" style="53" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
@@ -5158,249 +5158,315 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="49">
         <v>1</v>
       </c>
       <c r="B2">
         <v>2.2754067121320758E-2</v>
       </c>
-      <c r="F2" s="53"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>3.6777683199058619E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="49">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="53"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>5.6295732946324617E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="49">
         <v>3</v>
       </c>
       <c r="B4">
         <v>0.29049103768875639</v>
       </c>
-      <c r="F4" s="53"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>0.28018565116346822</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="49">
         <v>4</v>
       </c>
       <c r="B5">
         <v>6.8042645129231735E-2</v>
       </c>
-      <c r="F5" s="53"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>9.108448859608019E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="49">
         <v>5</v>
       </c>
       <c r="B6">
         <v>7.8129302482028457E-2</v>
       </c>
-      <c r="F6" s="53"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>7.5915521684292817E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="49">
         <v>6</v>
       </c>
       <c r="B7">
         <v>4.7497250824502138E-2</v>
       </c>
-      <c r="F7" s="53"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>6.3388027275901159E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="49">
         <v>7</v>
       </c>
       <c r="B8">
         <v>3.6338794222860751E-2</v>
       </c>
-      <c r="F8" s="53"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>2.1970540768343809E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="49">
         <v>8</v>
       </c>
       <c r="B9">
         <v>2.0662870555947292E-2</v>
       </c>
-      <c r="F9" s="53"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>4.882855601271921E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="49">
         <v>9</v>
       </c>
-      <c r="F10" s="53"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="49">
         <v>10</v>
       </c>
       <c r="B11">
         <v>3.0953547589416069E-2</v>
       </c>
-      <c r="F11" s="53"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>1.0264361308076749E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="49">
         <v>11</v>
       </c>
       <c r="B12">
         <v>7.4132979393461293E-2</v>
       </c>
-      <c r="F12" s="53"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>5.850408241707817E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="49">
         <v>12</v>
       </c>
       <c r="B13">
         <v>4.9246154578647311E-2</v>
       </c>
-      <c r="F13" s="53"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>2.784041719545963E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="49">
         <v>13</v>
       </c>
       <c r="B14">
         <v>1.965539608203001E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>5.1323973692984859E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="49">
         <v>14</v>
       </c>
       <c r="B15">
         <v>3.2389487339470467E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <v>4.6433748571819301E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="49">
         <v>15</v>
       </c>
       <c r="B16">
         <v>6.6570367082730827E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>4.4014910901996003E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="49">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="49">
         <v>17</v>
       </c>
       <c r="B18">
         <v>6.3629135804826223E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>3.2644514686287388E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="49">
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <v>2.6481671533126909E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="49">
         <v>19</v>
       </c>
       <c r="B20">
         <v>0.11848247807032609</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>3.4100794354838941E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="49">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <v>5.8719428050553413E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="49">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="49">
         <v>22</v>
       </c>
       <c r="B23">
         <v>1.993343775752613E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="49">
         <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <v>2.980599690868627E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="49">
         <v>24</v>
       </c>
       <c r="B25">
         <v>0.1951791960048343</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="49">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="49">
         <v>26</v>
       </c>
       <c r="B27">
         <v>3.2407550746685963E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <v>4.4046625330704393E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="49">
         <v>27</v>
       </c>
       <c r="B28">
         <v>3.4258050052886943E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <v>3.6462036747490233E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="49">
         <v>28</v>
       </c>
       <c r="B29">
         <v>6.8781449076960016E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <v>3.1613731843301768E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="49">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="49">
         <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <v>1.325813851648E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="49">
         <v>31</v>
       </c>
       <c r="B32">
         <v>0.1196731150278019</v>
+      </c>
+      <c r="C32">
+        <v>4.257717226305445E-2</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -5410,6 +5476,9 @@
       <c r="B33">
         <v>0.63103958284787054</v>
       </c>
+      <c r="C33" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="49">
@@ -5418,6 +5487,9 @@
       <c r="B34" t="s">
         <v>26</v>
       </c>
+      <c r="C34" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="49">
@@ -5426,6 +5498,9 @@
       <c r="B35" t="s">
         <v>26</v>
       </c>
+      <c r="C35" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="49">
@@ -5434,6 +5509,9 @@
       <c r="B36">
         <v>9.9464665623705234E-2</v>
       </c>
+      <c r="C36" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="50">
@@ -5442,6 +5520,9 @@
       <c r="B37">
         <v>2.5667307705730329E-2</v>
       </c>
+      <c r="C37" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="52" t="s">
@@ -5451,9 +5532,9 @@
         <f>SUBTOTAL(101,Tabel5[WiGLE: error of combination with highest RSSI])</f>
         <v>9.3557494533731536E-2</v>
       </c>
-      <c r="C38" t="e">
+      <c r="C38">
         <f>SUBTOTAL(101,Tabel5[LocationAPI: error of combination with highest RSSI2])</f>
-        <v>#DIV/0!</v>
+        <v>4.5829482412777948E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>